<commit_message>
Works when downloaded from fulcrum
</commit_message>
<xml_diff>
--- a/templates/PSE.xlsx
+++ b/templates/PSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Booker Engineering\CLIENTS\CABLECOM\POLE PERMITS\WOODINVILLE\JB0000965022_PSE_Pole Permit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04ef7c6c9ce6ee46/Documents/GitHub/pole-permit-spreadsheet/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DE45B7-B5AB-451E-AAEC-16ED1A4514A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{29DE45B7-B5AB-451E-AAEC-16ED1A4514A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{090D55B9-93FD-446D-9B69-9592C2A03785}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22764" yWindow="1104" windowWidth="21420" windowHeight="10356" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proposed Appendix A" sheetId="1" r:id="rId1"/>
@@ -86,12 +86,6 @@
     <t>City/Area</t>
   </si>
   <si>
-    <t xml:space="preserve">Neutral </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary </t>
-  </si>
-  <si>
     <t>Drip Loop</t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t xml:space="preserve">Address: </t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Secondary</t>
   </si>
 </sst>
 </file>
@@ -833,7 +833,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:N7"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -959,7 +959,7 @@
       </c>
       <c r="E5" s="39"/>
       <c r="F5" s="43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G5" s="38"/>
       <c r="H5" s="38"/>
@@ -1073,40 +1073,40 @@
         <v>15</v>
       </c>
       <c r="H9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="K9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="L9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="M9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="N9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="O9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="P9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="Q9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="10" t="s">
+      <c r="R9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Q9" s="11" t="s">
+      <c r="S9" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="R9" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="S9" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
@@ -4663,34 +4663,34 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C4" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C5" s="20" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>